<commit_message>
update BRD and BOM
</commit_message>
<xml_diff>
--- a/hardware/homegreen_node_basic v1.4.4 BOM.xlsx
+++ b/hardware/homegreen_node_basic v1.4.4 BOM.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmale/SourceTree/homegreen/Eagle/Node Basic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmale/SourceTree/homegreen-node/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812F5FAE-EB4A-8943-9D43-93C91660F02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34EBA75-F7A0-EC46-8CEF-4D233EC8BC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="homegreen_node_basic v1.4.2" sheetId="1" r:id="rId2"/>
+    <sheet name="BOM" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="homegreen_node_basic_v1.4.3" localSheetId="1">'homegreen_node_basic v1.4.2'!$A$34:$H$61</definedName>
-    <definedName name="homegreen_node_basic_v1.4.4" localSheetId="1">'homegreen_node_basic v1.4.2'!$A$2:$H$34</definedName>
+    <definedName name="homegreen_node_basic_v1.4.3" localSheetId="1">BOM!$A$34:$I$61</definedName>
+    <definedName name="homegreen_node_basic_v1.4.4" localSheetId="1">BOM!$A$2:$I$34</definedName>
     <definedName name="homegreen_node_basic_v1.4.4" localSheetId="0">Sheet1!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="212">
   <si>
     <t>Qty</t>
   </si>
@@ -722,6 +722,36 @@
   </si>
   <si>
     <t>https://lcsc.com/product-detail/DC-DC-Converters_XI-AN-Aerosemi-Tech-MT3608_C84817.html</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>bot</t>
+  </si>
+  <si>
+    <t>1xtop+9xbot</t>
+  </si>
+  <si>
+    <t>2xtop+4xbot</t>
+  </si>
+  <si>
+    <t>1xtop+1xbot</t>
+  </si>
+  <si>
+    <t>top 9pcbs</t>
+  </si>
+  <si>
+    <t>top 0</t>
+  </si>
+  <si>
+    <t>top 10 pcbs</t>
+  </si>
+  <si>
+    <t>0 Ohm R?</t>
   </si>
 </sst>
 </file>
@@ -870,7 +900,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1065,6 +1095,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1231,7 +1267,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1243,6 +1278,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1308,17 +1346,17 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="homegreen_node_basic v1.4.4" connectionId="3" xr16:uid="{0C86BC51-2716-9B43-8B71-99BCFEF6A804}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="homegreen_node_basic v1.4.3" connectionId="1" xr16:uid="{A604430B-28B8-4346-BCF2-C00A5E364440}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="homegreen_node_basic v1.4.4" connectionId="3" xr16:uid="{0C86BC51-2716-9B43-8B71-99BCFEF6A804}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1356,7 +1394,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1462,7 +1500,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1604,7 +1642,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2287,1112 +2325,1181 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="132" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="132" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.1640625" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="37.1640625" customWidth="1"/>
-    <col min="9" max="10" width="16.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="4" max="5" width="25.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="37.1640625" customWidth="1"/>
+    <col min="10" max="11" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>73</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>148</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2">
         <f>A2*30</f>
         <v>30</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="5">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>61400416021</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>61400416021</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>61400416021</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I34" si="0">A3*30</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J34" si="0">A3*30</f>
         <v>30</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="L3" s="1"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="L4" s="1"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="20">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>10</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="L5" s="1"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="L6" s="1"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="E7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="L7" s="1"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="L8" s="1"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="20">
-      <c r="A9" s="6">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="5">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="L9" s="1"/>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>6</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="L10" s="1"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="6">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="5">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="2">
         <v>100</v>
       </c>
-      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="5">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="4">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="L12" s="1"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="L13" s="1"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>2</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>47</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="L14" s="1"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="K15" s="3">
+      <c r="L15" s="2">
         <v>200</v>
       </c>
-      <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>4</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="5">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="L17" s="1"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>3</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="L18" s="1"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>2</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="L19" s="1"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="5">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="4">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="L20" s="1"/>
+      <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="5">
-        <v>1</v>
-      </c>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K21" s="3">
+      <c r="L21" s="2">
         <v>40</v>
       </c>
-      <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="5">
-        <v>1</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K22" s="3">
+      <c r="L22" s="2">
         <v>40</v>
       </c>
-      <c r="L22" s="1"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="5">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="L23" s="1"/>
+      <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="5">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="4">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="L24" s="1"/>
+      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="5">
-        <v>1</v>
-      </c>
-      <c r="B25" s="8" t="s">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K25" s="3">
+      <c r="L25" s="2">
         <v>50</v>
       </c>
-      <c r="L25" s="1"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="6">
-        <v>1</v>
-      </c>
-      <c r="B26" s="8" t="s">
+      <c r="A26" s="5">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="L26" s="1"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="5">
-        <v>1</v>
-      </c>
-      <c r="B27" s="8" t="s">
+      <c r="A27" s="4">
+        <v>1</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="L27" s="1"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:12" ht="20">
-      <c r="A28" s="5">
-        <v>1</v>
-      </c>
-      <c r="B28" s="8" t="s">
+      <c r="A28" s="4">
+        <v>1</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="L28" s="1"/>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="5">
-        <v>1</v>
-      </c>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="K29" s="3">
+      <c r="L29" s="2">
         <v>33</v>
       </c>
-      <c r="L29" s="1"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="6">
-        <v>1</v>
-      </c>
-      <c r="B30" s="8" t="s">
+      <c r="A30" s="5">
+        <v>1</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J30" s="3"/>
-      <c r="L30" s="1"/>
+      <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="5">
-        <v>1</v>
-      </c>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="H31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I31" s="1">
+      <c r="J31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="L31" s="1"/>
+      <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="6">
-        <v>1</v>
-      </c>
-      <c r="B32" s="8" t="s">
+      <c r="A32" s="5">
+        <v>1</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="6">
-        <v>1</v>
-      </c>
-      <c r="B33" s="8" t="s">
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="5">
+        <v>1</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="J33" s="3"/>
-      <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="6">
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="5">
         <v>2</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I34" s="1">
+      <c r="J34">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="J34" s="3"/>
-      <c r="L34" s="1"/>
+      <c r="K34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>